<commit_message>
Update webgame projectData and planning document
- Update kanji/apple/puzzle projectData with AI vibe coding terminology
- Update UndeadSurvivor planning document (Excel)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/assets/docs/UndeadSurvivor_기획서_박진.xlsx
+++ b/assets/docs/UndeadSurvivor_기획서_박진.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunbo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunbo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26445" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="로그라이트 프로젝트 기획서" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="328">
   <si>
     <t>1. 게임 개요</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1241,10 +1241,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4. 스탯 1개 Lv.10(MAX)기준 총 5,457G 필요 → 모든 스탯 최대 성장 불가, 선택 요구.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1. 웨이브 클리어시 골드와 보상 카드 선택권 지급</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1306,6 +1302,22 @@
   </si>
   <si>
     <t>없음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경제 밸런스 설계 의도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> - 플레이어가 1개 스탯을 끝까지 올릴지, 여러 스탯을 균등하게 투자할지 선택하도록 유도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. 스탯 1개 Lv.10(MAX)기준 총 5,457G 필요 → 9 웨이브 총 보상이 5,490G, 모든 스탯 최대 성장 불가. 투자 선택 요구.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> - 9웨이브 총 보상(5,490G)을 1개 스탯 MAX 비용(5,457G)의 근사치로 설계.  </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1854,7 +1866,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>502</xdr:row>
+      <xdr:row>497</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184731" cy="264560"/>
@@ -2420,13 +2432,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>117</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>121</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2436,8 +2448,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9591675" y="32499300"/>
-          <a:ext cx="4591050" cy="838200"/>
+          <a:off x="11602010" y="25814991"/>
+          <a:ext cx="4575362" cy="823072"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -2543,13 +2555,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>122</xdr:row>
+      <xdr:row>121</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>126</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2559,8 +2571,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9944100" y="33404175"/>
-          <a:ext cx="4591050" cy="838200"/>
+          <a:off x="11952194" y="26708100"/>
+          <a:ext cx="4575362" cy="1490382"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -2643,13 +2655,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>126</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>130</xdr:row>
+      <xdr:row>129</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2742,13 +2754,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>130</xdr:row>
+      <xdr:row>129</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>134</xdr:row>
+      <xdr:row>133</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2810,13 +2822,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>231322</xdr:colOff>
-      <xdr:row>120</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>149678</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>517072</xdr:colOff>
-      <xdr:row>123</xdr:row>
+      <xdr:row>122</xdr:row>
       <xdr:rowOff>136071</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2826,8 +2838,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13838465" y="32316964"/>
-          <a:ext cx="285750" cy="598714"/>
+          <a:off x="15941969" y="26393854"/>
+          <a:ext cx="285750" cy="625129"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
           <a:avLst/>
@@ -2873,13 +2885,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>574222</xdr:colOff>
-      <xdr:row>124</xdr:row>
+      <xdr:row>123</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>179615</xdr:colOff>
-      <xdr:row>127</xdr:row>
+      <xdr:row>126</xdr:row>
       <xdr:rowOff>138792</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2936,13 +2948,13 @@
     <xdr:from>
       <xdr:col>24</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>129</xdr:row>
+      <xdr:row>128</xdr:row>
       <xdr:rowOff>5443</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>131</xdr:row>
+      <xdr:row>130</xdr:row>
       <xdr:rowOff>195943</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5119,14 +5131,14 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>672354</xdr:colOff>
-      <xdr:row>142</xdr:row>
-      <xdr:rowOff>22417</xdr:rowOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>22414</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>462804</xdr:colOff>
-      <xdr:row>146</xdr:row>
-      <xdr:rowOff>19616</xdr:rowOff>
+      <xdr:row>143</xdr:row>
+      <xdr:rowOff>19613</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5135,7 +5147,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11609295" y="37797446"/>
+          <a:off x="11598089" y="30356738"/>
           <a:ext cx="4575362" cy="848846"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -5214,14 +5226,14 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>338979</xdr:colOff>
-      <xdr:row>146</xdr:row>
-      <xdr:rowOff>89653</xdr:rowOff>
+      <xdr:row>143</xdr:row>
+      <xdr:rowOff>89650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>129429</xdr:colOff>
-      <xdr:row>150</xdr:row>
-      <xdr:rowOff>89652</xdr:rowOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>89649</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5230,8 +5242,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11959479" y="38716329"/>
-          <a:ext cx="4575362" cy="851647"/>
+          <a:off x="11948273" y="31275621"/>
+          <a:ext cx="4575362" cy="851646"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -5371,14 +5383,14 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>643779</xdr:colOff>
-      <xdr:row>150</xdr:row>
-      <xdr:rowOff>156327</xdr:rowOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>156324</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>434229</xdr:colOff>
-      <xdr:row>162</xdr:row>
-      <xdr:rowOff>134471</xdr:rowOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5387,8 +5399,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12264279" y="39847562"/>
-          <a:ext cx="4575362" cy="2533085"/>
+          <a:off x="12196243" y="30976503"/>
+          <a:ext cx="4552950" cy="2660354"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -5563,14 +5575,14 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>227401</xdr:colOff>
-      <xdr:row>144</xdr:row>
-      <xdr:rowOff>201230</xdr:rowOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>201228</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>513151</xdr:colOff>
-      <xdr:row>147</xdr:row>
-      <xdr:rowOff>187623</xdr:rowOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>187621</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5579,7 +5591,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15949254" y="38402083"/>
+          <a:off x="15938048" y="30961375"/>
           <a:ext cx="285750" cy="625128"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
@@ -5626,14 +5638,14 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>570301</xdr:colOff>
-      <xdr:row>148</xdr:row>
-      <xdr:rowOff>203952</xdr:rowOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>203950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>175694</xdr:colOff>
-      <xdr:row>151</xdr:row>
-      <xdr:rowOff>190344</xdr:rowOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>190342</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5642,7 +5654,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16292154" y="39256452"/>
+          <a:off x="16280948" y="31815744"/>
           <a:ext cx="288952" cy="625127"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
@@ -5689,14 +5701,14 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>672354</xdr:colOff>
-      <xdr:row>169</xdr:row>
-      <xdr:rowOff>22417</xdr:rowOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>201711</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>462804</xdr:colOff>
-      <xdr:row>173</xdr:row>
-      <xdr:rowOff>19616</xdr:rowOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>198910</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5705,7 +5717,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11609295" y="38010358"/>
+          <a:off x="11598089" y="35690740"/>
           <a:ext cx="4575362" cy="848846"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -5795,14 +5807,14 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>338979</xdr:colOff>
-      <xdr:row>173</xdr:row>
-      <xdr:rowOff>89653</xdr:rowOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>56035</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>129429</xdr:colOff>
-      <xdr:row>177</xdr:row>
-      <xdr:rowOff>89648</xdr:rowOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>56030</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5811,7 +5823,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11959479" y="44722682"/>
+          <a:off x="11948273" y="36609623"/>
           <a:ext cx="4575362" cy="851642"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -5942,14 +5954,14 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>89646</xdr:colOff>
-      <xdr:row>177</xdr:row>
-      <xdr:rowOff>156327</xdr:rowOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>122709</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>445434</xdr:colOff>
-      <xdr:row>189</xdr:row>
-      <xdr:rowOff>134470</xdr:rowOff>
+      <xdr:row>185</xdr:row>
+      <xdr:rowOff>13607</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5958,8 +5970,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12393705" y="45641003"/>
-          <a:ext cx="4457141" cy="2533085"/>
+          <a:off x="12322467" y="36099995"/>
+          <a:ext cx="4437931" cy="2557898"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -6197,14 +6209,14 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>227401</xdr:colOff>
-      <xdr:row>171</xdr:row>
-      <xdr:rowOff>201230</xdr:rowOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>167612</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>513151</xdr:colOff>
-      <xdr:row>174</xdr:row>
-      <xdr:rowOff>187623</xdr:rowOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>154005</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6213,7 +6225,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15949254" y="38614995"/>
+          <a:off x="15938048" y="36295377"/>
           <a:ext cx="285750" cy="625128"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
@@ -6260,14 +6272,14 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>570301</xdr:colOff>
-      <xdr:row>175</xdr:row>
-      <xdr:rowOff>203952</xdr:rowOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>170334</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>175694</xdr:colOff>
-      <xdr:row>179</xdr:row>
-      <xdr:rowOff>190344</xdr:rowOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>156726</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6276,8 +6288,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16292154" y="39469364"/>
-          <a:ext cx="288952" cy="625127"/>
+          <a:off x="16280948" y="37149746"/>
+          <a:ext cx="288952" cy="838039"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
           <a:avLst/>
@@ -6323,13 +6335,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>33612</xdr:colOff>
-      <xdr:row>278</xdr:row>
+      <xdr:row>273</xdr:row>
       <xdr:rowOff>201706</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>33612</xdr:colOff>
-      <xdr:row>283</xdr:row>
+      <xdr:row>278</xdr:row>
       <xdr:rowOff>123265</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6390,13 +6402,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>533396</xdr:colOff>
-      <xdr:row>278</xdr:row>
+      <xdr:row>273</xdr:row>
       <xdr:rowOff>197224</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>533397</xdr:colOff>
-      <xdr:row>283</xdr:row>
+      <xdr:row>278</xdr:row>
       <xdr:rowOff>118783</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6457,13 +6469,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>304797</xdr:colOff>
-      <xdr:row>278</xdr:row>
+      <xdr:row>273</xdr:row>
       <xdr:rowOff>192742</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>304797</xdr:colOff>
-      <xdr:row>283</xdr:row>
+      <xdr:row>278</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6528,13 +6540,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>42579</xdr:colOff>
-      <xdr:row>278</xdr:row>
+      <xdr:row>273</xdr:row>
       <xdr:rowOff>199466</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>42580</xdr:colOff>
-      <xdr:row>283</xdr:row>
+      <xdr:row>278</xdr:row>
       <xdr:rowOff>121025</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6595,13 +6607,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>33612</xdr:colOff>
-      <xdr:row>281</xdr:row>
+      <xdr:row>276</xdr:row>
       <xdr:rowOff>51547</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>533396</xdr:colOff>
-      <xdr:row>281</xdr:row>
+      <xdr:row>276</xdr:row>
       <xdr:rowOff>56029</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -6645,13 +6657,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>533397</xdr:colOff>
-      <xdr:row>281</xdr:row>
+      <xdr:row>276</xdr:row>
       <xdr:rowOff>47065</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>304797</xdr:colOff>
-      <xdr:row>281</xdr:row>
+      <xdr:row>276</xdr:row>
       <xdr:rowOff>51547</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -6695,13 +6707,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>304797</xdr:colOff>
-      <xdr:row>281</xdr:row>
+      <xdr:row>276</xdr:row>
       <xdr:rowOff>47065</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>42579</xdr:colOff>
-      <xdr:row>281</xdr:row>
+      <xdr:row>276</xdr:row>
       <xdr:rowOff>53789</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -6745,13 +6757,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>224117</xdr:colOff>
-      <xdr:row>249</xdr:row>
+      <xdr:row>244</xdr:row>
       <xdr:rowOff>44823</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>224118</xdr:colOff>
-      <xdr:row>252</xdr:row>
+      <xdr:row>247</xdr:row>
       <xdr:rowOff>24865</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6818,13 +6830,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>224118</xdr:colOff>
-      <xdr:row>250</xdr:row>
+      <xdr:row>245</xdr:row>
       <xdr:rowOff>133725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>324971</xdr:colOff>
-      <xdr:row>250</xdr:row>
+      <xdr:row>245</xdr:row>
       <xdr:rowOff>141300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -6868,13 +6880,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>324971</xdr:colOff>
-      <xdr:row>248</xdr:row>
+      <xdr:row>243</xdr:row>
       <xdr:rowOff>33619</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>324972</xdr:colOff>
-      <xdr:row>253</xdr:row>
+      <xdr:row>248</xdr:row>
       <xdr:rowOff>32125</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6941,13 +6953,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>605117</xdr:colOff>
-      <xdr:row>247</xdr:row>
+      <xdr:row>242</xdr:row>
       <xdr:rowOff>144078</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>139274</xdr:colOff>
-      <xdr:row>253</xdr:row>
+      <xdr:row>248</xdr:row>
       <xdr:rowOff>116860</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7008,13 +7020,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>324972</xdr:colOff>
-      <xdr:row>250</xdr:row>
+      <xdr:row>245</xdr:row>
       <xdr:rowOff>124866</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>605117</xdr:colOff>
-      <xdr:row>250</xdr:row>
+      <xdr:row>245</xdr:row>
       <xdr:rowOff>133725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7058,13 +7070,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>526675</xdr:colOff>
-      <xdr:row>253</xdr:row>
+      <xdr:row>248</xdr:row>
       <xdr:rowOff>111045</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>526675</xdr:colOff>
-      <xdr:row>255</xdr:row>
+      <xdr:row>250</xdr:row>
       <xdr:rowOff>322462</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7175,13 +7187,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>139274</xdr:colOff>
-      <xdr:row>250</xdr:row>
+      <xdr:row>245</xdr:row>
       <xdr:rowOff>124866</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>526675</xdr:colOff>
-      <xdr:row>255</xdr:row>
+      <xdr:row>250</xdr:row>
       <xdr:rowOff>3842</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7225,13 +7237,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>139274</xdr:colOff>
-      <xdr:row>243</xdr:row>
+      <xdr:row>238</xdr:row>
       <xdr:rowOff>193754</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>590711</xdr:colOff>
-      <xdr:row>250</xdr:row>
+      <xdr:row>245</xdr:row>
       <xdr:rowOff>124866</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7275,13 +7287,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>590711</xdr:colOff>
-      <xdr:row>242</xdr:row>
+      <xdr:row>237</xdr:row>
       <xdr:rowOff>88045</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>590709</xdr:colOff>
-      <xdr:row>245</xdr:row>
+      <xdr:row>240</xdr:row>
       <xdr:rowOff>86551</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7392,13 +7404,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>358588</xdr:colOff>
-      <xdr:row>253</xdr:row>
+      <xdr:row>248</xdr:row>
       <xdr:rowOff>116918</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>358588</xdr:colOff>
-      <xdr:row>255</xdr:row>
+      <xdr:row>250</xdr:row>
       <xdr:rowOff>328922</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7465,13 +7477,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>238952</xdr:colOff>
-      <xdr:row>253</xdr:row>
+      <xdr:row>248</xdr:row>
       <xdr:rowOff>118464</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>238952</xdr:colOff>
-      <xdr:row>255</xdr:row>
+      <xdr:row>250</xdr:row>
       <xdr:rowOff>329881</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7614,13 +7626,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>526675</xdr:colOff>
-      <xdr:row>255</xdr:row>
+      <xdr:row>250</xdr:row>
       <xdr:rowOff>3842</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>358588</xdr:colOff>
-      <xdr:row>255</xdr:row>
+      <xdr:row>250</xdr:row>
       <xdr:rowOff>10008</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7664,13 +7676,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>358588</xdr:colOff>
-      <xdr:row>255</xdr:row>
+      <xdr:row>250</xdr:row>
       <xdr:rowOff>10008</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>238952</xdr:colOff>
-      <xdr:row>255</xdr:row>
+      <xdr:row>250</xdr:row>
       <xdr:rowOff>11261</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7714,13 +7726,13 @@
     <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>132496</xdr:colOff>
-      <xdr:row>253</xdr:row>
+      <xdr:row>248</xdr:row>
       <xdr:rowOff>111260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>132496</xdr:colOff>
-      <xdr:row>255</xdr:row>
+      <xdr:row>250</xdr:row>
       <xdr:rowOff>334470</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7839,13 +7851,13 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>238952</xdr:colOff>
-      <xdr:row>255</xdr:row>
+      <xdr:row>250</xdr:row>
       <xdr:rowOff>9953</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>132496</xdr:colOff>
-      <xdr:row>255</xdr:row>
+      <xdr:row>250</xdr:row>
       <xdr:rowOff>11261</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7889,13 +7901,13 @@
     <xdr:from>
       <xdr:col>24</xdr:col>
       <xdr:colOff>132496</xdr:colOff>
-      <xdr:row>254</xdr:row>
+      <xdr:row>249</xdr:row>
       <xdr:rowOff>160953</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>44823</xdr:colOff>
-      <xdr:row>254</xdr:row>
+      <xdr:row>249</xdr:row>
       <xdr:rowOff>165849</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7939,13 +7951,13 @@
     <xdr:from>
       <xdr:col>25</xdr:col>
       <xdr:colOff>44823</xdr:colOff>
-      <xdr:row>251</xdr:row>
+      <xdr:row>246</xdr:row>
       <xdr:rowOff>176893</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>262539</xdr:colOff>
-      <xdr:row>257</xdr:row>
+      <xdr:row>252</xdr:row>
       <xdr:rowOff>154804</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -8029,13 +8041,13 @@
     <xdr:from>
       <xdr:col>40</xdr:col>
       <xdr:colOff>9551</xdr:colOff>
-      <xdr:row>253</xdr:row>
+      <xdr:row>248</xdr:row>
       <xdr:rowOff>138097</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>9552</xdr:colOff>
-      <xdr:row>255</xdr:row>
+      <xdr:row>250</xdr:row>
       <xdr:rowOff>341297</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -8102,13 +8114,13 @@
     <xdr:from>
       <xdr:col>27</xdr:col>
       <xdr:colOff>262539</xdr:colOff>
-      <xdr:row>254</xdr:row>
+      <xdr:row>249</xdr:row>
       <xdr:rowOff>165849</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>162486</xdr:colOff>
-      <xdr:row>254</xdr:row>
+      <xdr:row>249</xdr:row>
       <xdr:rowOff>165901</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8152,13 +8164,13 @@
     <xdr:from>
       <xdr:col>29</xdr:col>
       <xdr:colOff>162486</xdr:colOff>
-      <xdr:row>253</xdr:row>
+      <xdr:row>248</xdr:row>
       <xdr:rowOff>122945</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
       <xdr:colOff>162486</xdr:colOff>
-      <xdr:row>255</xdr:row>
+      <xdr:row>250</xdr:row>
       <xdr:rowOff>323156</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -8225,13 +8237,13 @@
     <xdr:from>
       <xdr:col>32</xdr:col>
       <xdr:colOff>156882</xdr:colOff>
-      <xdr:row>251</xdr:row>
+      <xdr:row>246</xdr:row>
       <xdr:rowOff>194183</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
       <xdr:colOff>374598</xdr:colOff>
-      <xdr:row>257</xdr:row>
+      <xdr:row>252</xdr:row>
       <xdr:rowOff>163287</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -8315,13 +8327,13 @@
     <xdr:from>
       <xdr:col>31</xdr:col>
       <xdr:colOff>162486</xdr:colOff>
-      <xdr:row>254</xdr:row>
+      <xdr:row>249</xdr:row>
       <xdr:rowOff>165901</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
       <xdr:colOff>156882</xdr:colOff>
-      <xdr:row>254</xdr:row>
+      <xdr:row>249</xdr:row>
       <xdr:rowOff>178735</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8365,13 +8377,13 @@
     <xdr:from>
       <xdr:col>34</xdr:col>
       <xdr:colOff>374598</xdr:colOff>
-      <xdr:row>254</xdr:row>
+      <xdr:row>249</xdr:row>
       <xdr:rowOff>178735</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
       <xdr:colOff>590709</xdr:colOff>
-      <xdr:row>254</xdr:row>
+      <xdr:row>249</xdr:row>
       <xdr:rowOff>197744</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8415,13 +8427,13 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>590709</xdr:colOff>
-      <xdr:row>253</xdr:row>
+      <xdr:row>248</xdr:row>
       <xdr:rowOff>181376</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>616109</xdr:colOff>
-      <xdr:row>255</xdr:row>
+      <xdr:row>250</xdr:row>
       <xdr:rowOff>299837</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -8488,13 +8500,13 @@
     <xdr:from>
       <xdr:col>38</xdr:col>
       <xdr:colOff>616109</xdr:colOff>
-      <xdr:row>255</xdr:row>
+      <xdr:row>250</xdr:row>
       <xdr:rowOff>26785</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
       <xdr:colOff>9551</xdr:colOff>
-      <xdr:row>255</xdr:row>
+      <xdr:row>250</xdr:row>
       <xdr:rowOff>27695</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8538,13 +8550,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>263740</xdr:colOff>
-      <xdr:row>253</xdr:row>
+      <xdr:row>248</xdr:row>
       <xdr:rowOff>32125</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>153681</xdr:colOff>
-      <xdr:row>257</xdr:row>
+      <xdr:row>252</xdr:row>
       <xdr:rowOff>154804</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8596,13 +8608,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>590711</xdr:colOff>
-      <xdr:row>245</xdr:row>
+      <xdr:row>240</xdr:row>
       <xdr:rowOff>86551</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
       <xdr:colOff>265741</xdr:colOff>
-      <xdr:row>251</xdr:row>
+      <xdr:row>246</xdr:row>
       <xdr:rowOff>194183</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8654,13 +8666,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>590709</xdr:colOff>
-      <xdr:row>243</xdr:row>
+      <xdr:row>238</xdr:row>
       <xdr:rowOff>193754</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>453841</xdr:colOff>
-      <xdr:row>243</xdr:row>
+      <xdr:row>238</xdr:row>
       <xdr:rowOff>196286</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8704,13 +8716,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>453841</xdr:colOff>
-      <xdr:row>239</xdr:row>
+      <xdr:row>234</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>174494</xdr:colOff>
-      <xdr:row>247</xdr:row>
+      <xdr:row>242</xdr:row>
       <xdr:rowOff>202072</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -8810,13 +8822,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>324972</xdr:colOff>
-      <xdr:row>239</xdr:row>
+      <xdr:row>234</xdr:row>
       <xdr:rowOff>190498</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>655947</xdr:colOff>
-      <xdr:row>248</xdr:row>
+      <xdr:row>243</xdr:row>
       <xdr:rowOff>33618</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8868,13 +8880,13 @@
     <xdr:from>
       <xdr:col>20</xdr:col>
       <xdr:colOff>174494</xdr:colOff>
-      <xdr:row>243</xdr:row>
+      <xdr:row>238</xdr:row>
       <xdr:rowOff>196286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>41</xdr:col>
       <xdr:colOff>9552</xdr:colOff>
-      <xdr:row>253</xdr:row>
+      <xdr:row>248</xdr:row>
       <xdr:rowOff>138097</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8921,13 +8933,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>549088</xdr:colOff>
-      <xdr:row>325</xdr:row>
+      <xdr:row>320</xdr:row>
       <xdr:rowOff>89646</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>339539</xdr:colOff>
-      <xdr:row>329</xdr:row>
+      <xdr:row>324</xdr:row>
       <xdr:rowOff>61071</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -9041,13 +9053,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>215714</xdr:colOff>
-      <xdr:row>329</xdr:row>
+      <xdr:row>324</xdr:row>
       <xdr:rowOff>131108</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>6164</xdr:colOff>
-      <xdr:row>335</xdr:row>
+      <xdr:row>330</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -9089,7 +9101,7 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
@@ -9267,13 +9279,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>554132</xdr:colOff>
-      <xdr:row>335</xdr:row>
+      <xdr:row>330</xdr:row>
       <xdr:rowOff>63313</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>344582</xdr:colOff>
-      <xdr:row>342</xdr:row>
+      <xdr:row>337</xdr:row>
       <xdr:rowOff>67235</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -9315,7 +9327,7 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
@@ -9446,13 +9458,13 @@
     <xdr:from>
       <xdr:col>20</xdr:col>
       <xdr:colOff>104136</xdr:colOff>
-      <xdr:row>328</xdr:row>
+      <xdr:row>323</xdr:row>
       <xdr:rowOff>29775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>389886</xdr:colOff>
-      <xdr:row>331</xdr:row>
+      <xdr:row>326</xdr:row>
       <xdr:rowOff>16168</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -9509,13 +9521,13 @@
     <xdr:from>
       <xdr:col>20</xdr:col>
       <xdr:colOff>447036</xdr:colOff>
-      <xdr:row>333</xdr:row>
+      <xdr:row>328</xdr:row>
       <xdr:rowOff>110938</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>52429</xdr:colOff>
-      <xdr:row>336</xdr:row>
+      <xdr:row>331</xdr:row>
       <xdr:rowOff>97330</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -9572,13 +9584,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>44823</xdr:colOff>
-      <xdr:row>291</xdr:row>
+      <xdr:row>286</xdr:row>
       <xdr:rowOff>100853</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>605119</xdr:colOff>
-      <xdr:row>296</xdr:row>
+      <xdr:row>291</xdr:row>
       <xdr:rowOff>11207</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -9639,13 +9651,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>145677</xdr:colOff>
-      <xdr:row>287</xdr:row>
+      <xdr:row>282</xdr:row>
       <xdr:rowOff>179293</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>145678</xdr:colOff>
-      <xdr:row>299</xdr:row>
+      <xdr:row>294</xdr:row>
       <xdr:rowOff>145675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -9841,13 +9853,13 @@
     <xdr:from>
       <xdr:col>26</xdr:col>
       <xdr:colOff>582709</xdr:colOff>
-      <xdr:row>287</xdr:row>
+      <xdr:row>282</xdr:row>
       <xdr:rowOff>112059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>459446</xdr:colOff>
-      <xdr:row>292</xdr:row>
+      <xdr:row>287</xdr:row>
       <xdr:rowOff>33619</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -9931,13 +9943,13 @@
     <xdr:from>
       <xdr:col>26</xdr:col>
       <xdr:colOff>582710</xdr:colOff>
-      <xdr:row>295</xdr:row>
+      <xdr:row>290</xdr:row>
       <xdr:rowOff>56028</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>459447</xdr:colOff>
-      <xdr:row>299</xdr:row>
+      <xdr:row>294</xdr:row>
       <xdr:rowOff>179293</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -9998,13 +10010,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>605119</xdr:colOff>
-      <xdr:row>293</xdr:row>
+      <xdr:row>288</xdr:row>
       <xdr:rowOff>168089</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>145677</xdr:colOff>
-      <xdr:row>293</xdr:row>
+      <xdr:row>288</xdr:row>
       <xdr:rowOff>173691</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -10048,13 +10060,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>661147</xdr:colOff>
-      <xdr:row>368</xdr:row>
+      <xdr:row>363</xdr:row>
       <xdr:rowOff>67235</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>425825</xdr:colOff>
-      <xdr:row>372</xdr:row>
+      <xdr:row>367</xdr:row>
       <xdr:rowOff>201705</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -10115,13 +10127,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>425825</xdr:colOff>
-      <xdr:row>370</xdr:row>
+      <xdr:row>365</xdr:row>
       <xdr:rowOff>134470</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>224118</xdr:colOff>
-      <xdr:row>370</xdr:row>
+      <xdr:row>365</xdr:row>
       <xdr:rowOff>134470</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -10165,13 +10177,13 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>526678</xdr:colOff>
-      <xdr:row>289</xdr:row>
+      <xdr:row>284</xdr:row>
       <xdr:rowOff>134471</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>481853</xdr:colOff>
-      <xdr:row>297</xdr:row>
+      <xdr:row>292</xdr:row>
       <xdr:rowOff>201706</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -10232,13 +10244,13 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>145678</xdr:colOff>
-      <xdr:row>293</xdr:row>
+      <xdr:row>288</xdr:row>
       <xdr:rowOff>173691</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>526678</xdr:colOff>
-      <xdr:row>293</xdr:row>
+      <xdr:row>288</xdr:row>
       <xdr:rowOff>173692</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -10282,13 +10294,13 @@
     <xdr:from>
       <xdr:col>24</xdr:col>
       <xdr:colOff>481853</xdr:colOff>
-      <xdr:row>289</xdr:row>
+      <xdr:row>284</xdr:row>
       <xdr:rowOff>179295</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>582709</xdr:colOff>
-      <xdr:row>293</xdr:row>
+      <xdr:row>288</xdr:row>
       <xdr:rowOff>173692</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -10335,13 +10347,13 @@
     <xdr:from>
       <xdr:col>24</xdr:col>
       <xdr:colOff>481853</xdr:colOff>
-      <xdr:row>293</xdr:row>
+      <xdr:row>288</xdr:row>
       <xdr:rowOff>173692</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>582710</xdr:colOff>
-      <xdr:row>297</xdr:row>
+      <xdr:row>292</xdr:row>
       <xdr:rowOff>123264</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -10388,13 +10400,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>89646</xdr:colOff>
-      <xdr:row>366</xdr:row>
+      <xdr:row>361</xdr:row>
       <xdr:rowOff>100854</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>44822</xdr:colOff>
-      <xdr:row>374</xdr:row>
+      <xdr:row>369</xdr:row>
       <xdr:rowOff>168089</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -10455,13 +10467,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>224118</xdr:colOff>
-      <xdr:row>368</xdr:row>
+      <xdr:row>363</xdr:row>
       <xdr:rowOff>67235</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>100855</xdr:colOff>
-      <xdr:row>372</xdr:row>
+      <xdr:row>367</xdr:row>
       <xdr:rowOff>201705</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -10545,13 +10557,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>100855</xdr:colOff>
-      <xdr:row>370</xdr:row>
+      <xdr:row>365</xdr:row>
       <xdr:rowOff>128869</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>89646</xdr:colOff>
-      <xdr:row>370</xdr:row>
+      <xdr:row>365</xdr:row>
       <xdr:rowOff>134470</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -10595,13 +10607,13 @@
     <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>621930</xdr:colOff>
-      <xdr:row>361</xdr:row>
+      <xdr:row>356</xdr:row>
       <xdr:rowOff>174493</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>498667</xdr:colOff>
-      <xdr:row>366</xdr:row>
+      <xdr:row>361</xdr:row>
       <xdr:rowOff>91250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -10693,13 +10705,13 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>44822</xdr:colOff>
-      <xdr:row>364</xdr:row>
+      <xdr:row>359</xdr:row>
       <xdr:rowOff>24015</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>621930</xdr:colOff>
-      <xdr:row>370</xdr:row>
+      <xdr:row>365</xdr:row>
       <xdr:rowOff>127669</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -10746,13 +10758,13 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>44822</xdr:colOff>
-      <xdr:row>370</xdr:row>
+      <xdr:row>365</xdr:row>
       <xdr:rowOff>128869</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>425822</xdr:colOff>
-      <xdr:row>377</xdr:row>
+      <xdr:row>372</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -10799,13 +10811,13 @@
     <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>425822</xdr:colOff>
-      <xdr:row>371</xdr:row>
+      <xdr:row>366</xdr:row>
       <xdr:rowOff>78441</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>380999</xdr:colOff>
-      <xdr:row>382</xdr:row>
+      <xdr:row>377</xdr:row>
       <xdr:rowOff>145677</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -10972,13 +10984,13 @@
     <xdr:from>
       <xdr:col>26</xdr:col>
       <xdr:colOff>380999</xdr:colOff>
-      <xdr:row>372</xdr:row>
+      <xdr:row>367</xdr:row>
       <xdr:rowOff>112059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>224118</xdr:colOff>
-      <xdr:row>377</xdr:row>
+      <xdr:row>372</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -11025,13 +11037,13 @@
     <xdr:from>
       <xdr:col>26</xdr:col>
       <xdr:colOff>380999</xdr:colOff>
-      <xdr:row>377</xdr:row>
+      <xdr:row>372</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>212912</xdr:colOff>
-      <xdr:row>381</xdr:row>
+      <xdr:row>376</xdr:row>
       <xdr:rowOff>56031</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -11078,13 +11090,13 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>224118</xdr:colOff>
-      <xdr:row>370</xdr:row>
+      <xdr:row>365</xdr:row>
       <xdr:rowOff>44824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
       <xdr:colOff>100854</xdr:colOff>
-      <xdr:row>374</xdr:row>
+      <xdr:row>369</xdr:row>
       <xdr:rowOff>179295</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -11145,13 +11157,13 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>212912</xdr:colOff>
-      <xdr:row>378</xdr:row>
+      <xdr:row>373</xdr:row>
       <xdr:rowOff>201707</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
       <xdr:colOff>89648</xdr:colOff>
-      <xdr:row>383</xdr:row>
+      <xdr:row>378</xdr:row>
       <xdr:rowOff>112060</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -11280,13 +11292,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>665150</xdr:colOff>
-      <xdr:row>403</xdr:row>
+      <xdr:row>398</xdr:row>
       <xdr:rowOff>172078</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>429828</xdr:colOff>
-      <xdr:row>408</xdr:row>
+      <xdr:row>403</xdr:row>
       <xdr:rowOff>88834</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -11363,13 +11375,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>429828</xdr:colOff>
-      <xdr:row>406</xdr:row>
+      <xdr:row>401</xdr:row>
       <xdr:rowOff>33218</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>165685</xdr:colOff>
-      <xdr:row>406</xdr:row>
+      <xdr:row>401</xdr:row>
       <xdr:rowOff>35206</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -11413,13 +11425,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>165685</xdr:colOff>
-      <xdr:row>403</xdr:row>
+      <xdr:row>398</xdr:row>
       <xdr:rowOff>68037</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>42422</xdr:colOff>
-      <xdr:row>408</xdr:row>
+      <xdr:row>403</xdr:row>
       <xdr:rowOff>188900</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -11524,13 +11536,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>631050</xdr:colOff>
-      <xdr:row>403</xdr:row>
+      <xdr:row>398</xdr:row>
       <xdr:rowOff>70758</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>507786</xdr:colOff>
-      <xdr:row>408</xdr:row>
+      <xdr:row>403</xdr:row>
       <xdr:rowOff>191621</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -11666,13 +11678,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>42422</xdr:colOff>
-      <xdr:row>406</xdr:row>
+      <xdr:row>401</xdr:row>
       <xdr:rowOff>33218</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>631050</xdr:colOff>
-      <xdr:row>406</xdr:row>
+      <xdr:row>401</xdr:row>
       <xdr:rowOff>35939</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -11716,13 +11728,13 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>470486</xdr:colOff>
-      <xdr:row>403</xdr:row>
+      <xdr:row>398</xdr:row>
       <xdr:rowOff>59873</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>347223</xdr:colOff>
-      <xdr:row>408</xdr:row>
+      <xdr:row>403</xdr:row>
       <xdr:rowOff>180736</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -11822,13 +11834,13 @@
     <xdr:from>
       <xdr:col>20</xdr:col>
       <xdr:colOff>507786</xdr:colOff>
-      <xdr:row>406</xdr:row>
+      <xdr:row>401</xdr:row>
       <xdr:rowOff>25054</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>470486</xdr:colOff>
-      <xdr:row>406</xdr:row>
+      <xdr:row>401</xdr:row>
       <xdr:rowOff>35939</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -11872,13 +11884,13 @@
     <xdr:from>
       <xdr:col>25</xdr:col>
       <xdr:colOff>367394</xdr:colOff>
-      <xdr:row>402</xdr:row>
+      <xdr:row>397</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>322570</xdr:colOff>
-      <xdr:row>410</xdr:row>
+      <xdr:row>405</xdr:row>
       <xdr:rowOff>53628</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -11962,13 +11974,13 @@
     <xdr:from>
       <xdr:col>24</xdr:col>
       <xdr:colOff>347223</xdr:colOff>
-      <xdr:row>406</xdr:row>
+      <xdr:row>401</xdr:row>
       <xdr:rowOff>25054</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>367394</xdr:colOff>
-      <xdr:row>406</xdr:row>
+      <xdr:row>401</xdr:row>
       <xdr:rowOff>26814</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -12012,13 +12024,13 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>322570</xdr:colOff>
-      <xdr:row>402</xdr:row>
+      <xdr:row>397</xdr:row>
       <xdr:rowOff>562</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>568458</xdr:colOff>
-      <xdr:row>406</xdr:row>
+      <xdr:row>401</xdr:row>
       <xdr:rowOff>26814</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -12062,13 +12074,13 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>322570</xdr:colOff>
-      <xdr:row>406</xdr:row>
+      <xdr:row>401</xdr:row>
       <xdr:rowOff>26814</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>598393</xdr:colOff>
-      <xdr:row>410</xdr:row>
+      <xdr:row>405</xdr:row>
       <xdr:rowOff>152962</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -12112,13 +12124,13 @@
     <xdr:from>
       <xdr:col>30</xdr:col>
       <xdr:colOff>568458</xdr:colOff>
-      <xdr:row>399</xdr:row>
+      <xdr:row>394</xdr:row>
       <xdr:rowOff>35380</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
       <xdr:colOff>445194</xdr:colOff>
-      <xdr:row>404</xdr:row>
+      <xdr:row>399</xdr:row>
       <xdr:rowOff>156244</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -12184,13 +12196,13 @@
     <xdr:from>
       <xdr:col>30</xdr:col>
       <xdr:colOff>598393</xdr:colOff>
-      <xdr:row>407</xdr:row>
+      <xdr:row>402</xdr:row>
       <xdr:rowOff>201387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
       <xdr:colOff>475129</xdr:colOff>
-      <xdr:row>413</xdr:row>
+      <xdr:row>408</xdr:row>
       <xdr:rowOff>118143</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -12610,10 +12622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:BA422"/>
+  <dimension ref="C3:BA417"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A400" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I426" sqref="I426"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C187" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -13197,232 +13209,294 @@
         <v>304</v>
       </c>
     </row>
-    <row r="117" spans="4:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="D117" s="25" t="s">
+    <row r="116" spans="4:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="D116" s="25" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D119" s="12" t="s">
+    <row r="118" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D118" s="12" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D120" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="121" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D121" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="122" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D122" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="123" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D123" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D124" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D126" s="12" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="125" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D125" s="12" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="127" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D127" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="128" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D128" t="s">
-        <v>62</v>
+        <v>302</v>
       </c>
     </row>
     <row r="129" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D129" t="s">
-        <v>302</v>
+        <v>63</v>
       </c>
     </row>
     <row r="130" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D130" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D131" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="132" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D132" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="133" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D133" t="s">
-        <v>65</v>
+        <v>318</v>
       </c>
     </row>
     <row r="134" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D134" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D135" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="141" spans="4:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="D141" s="25" t="s">
+    <row r="139" spans="4:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="D139" s="25" t="s">
         <v>67</v>
       </c>
     </row>
+    <row r="141" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D141" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
     <row r="143" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D143" s="12" t="s">
-        <v>68</v>
+      <c r="D143" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="144" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D144" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="145" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D145" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
     </row>
     <row r="146" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D146" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D147" t="s">
-        <v>287</v>
+        <v>309</v>
       </c>
     </row>
     <row r="148" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D148" t="s">
-        <v>310</v>
+      <c r="D148" s="12" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="150" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D150" s="12" t="s">
-        <v>320</v>
+      <c r="D150" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="151" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D151" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="152" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D152" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="153" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D153" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D154" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="155" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D155" t="s">
-        <v>72</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D156" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="157" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D157" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="158" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D158" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="159" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D159" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="160" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D160" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="168" spans="4:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="D168" s="25" t="s">
+    <row r="163" spans="4:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="D163" s="25" t="s">
         <v>288</v>
       </c>
     </row>
+    <row r="165" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D165" s="12" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="167" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D167" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="168" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D168" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="169" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D169" t="s">
+        <v>311</v>
+      </c>
+    </row>
     <row r="170" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D170" s="12" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="172" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D172" t="s">
-        <v>311</v>
+      <c r="D170" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="171" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D171" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="173" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D173" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="174" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D174" t="s">
-        <v>312</v>
+      <c r="D173" s="12" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="175" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D175" t="s">
-        <v>291</v>
+        <v>62</v>
       </c>
     </row>
     <row r="176" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D176" t="s">
-        <v>313</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="177" spans="3:38" x14ac:dyDescent="0.3">
+      <c r="D177" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="178" spans="3:38" x14ac:dyDescent="0.3">
-      <c r="D178" s="12" t="s">
-        <v>292</v>
+      <c r="D178" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="180" spans="3:38" x14ac:dyDescent="0.3">
       <c r="D180" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="181" spans="3:38" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="181" spans="3:38" ht="17.25" x14ac:dyDescent="0.3">
       <c r="D181" t="s">
-        <v>76</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="AA181" s="26"/>
+      <c r="AB181" s="1"/>
+      <c r="AC181" s="1"/>
+      <c r="AE181" s="1"/>
+      <c r="AF181" s="1"/>
+      <c r="AG181" s="1"/>
+      <c r="AH181" s="1"/>
     </row>
     <row r="182" spans="3:38" x14ac:dyDescent="0.3">
       <c r="D182" t="s">
-        <v>77</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="AA182" s="1"/>
+      <c r="AB182" s="1"/>
+      <c r="AC182" s="1"/>
+      <c r="AD182" s="1"/>
+      <c r="AE182" s="1"/>
+      <c r="AF182" s="1"/>
+      <c r="AG182" s="1"/>
+      <c r="AH182" s="1"/>
     </row>
     <row r="183" spans="3:38" x14ac:dyDescent="0.3">
       <c r="D183" t="s">
-        <v>80</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="AA183" s="1"/>
+      <c r="AB183" s="1"/>
+      <c r="AC183" s="1"/>
+      <c r="AD183" s="1"/>
+      <c r="AE183" s="1"/>
+      <c r="AF183" s="1"/>
+      <c r="AG183" s="1"/>
+      <c r="AH183" s="1"/>
+    </row>
+    <row r="184" spans="3:38" x14ac:dyDescent="0.3">
+      <c r="AJ184" s="1"/>
+      <c r="AK184" s="1"/>
+      <c r="AL184" s="1"/>
     </row>
     <row r="185" spans="3:38" x14ac:dyDescent="0.3">
-      <c r="D185" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="186" spans="3:38" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D186" t="s">
-        <v>293</v>
-      </c>
-      <c r="AA186" s="26"/>
-      <c r="AB186" s="1"/>
-      <c r="AC186" s="1"/>
-      <c r="AE186" s="1"/>
-      <c r="AF186" s="1"/>
-      <c r="AG186" s="1"/>
-      <c r="AH186" s="1"/>
+      <c r="AJ185" s="1"/>
+      <c r="AK185" s="1"/>
+      <c r="AL185" s="1"/>
+    </row>
+    <row r="186" spans="3:38" x14ac:dyDescent="0.3">
+      <c r="AJ186" s="1"/>
+      <c r="AK186" s="1"/>
+      <c r="AL186" s="1"/>
     </row>
     <row r="187" spans="3:38" x14ac:dyDescent="0.3">
-      <c r="D187" t="s">
-        <v>78</v>
-      </c>
+      <c r="C187" s="1"/>
+      <c r="D187" s="1"/>
+      <c r="E187" s="1"/>
+      <c r="F187" s="1"/>
+      <c r="G187" s="1"/>
+      <c r="H187" s="1"/>
+      <c r="I187" s="1"/>
+      <c r="J187" s="1"/>
+      <c r="K187" s="1"/>
+      <c r="L187" s="1"/>
+      <c r="M187" s="1"/>
+      <c r="N187" s="1"/>
+      <c r="O187" s="1"/>
+      <c r="P187" s="1"/>
+      <c r="Q187" s="1"/>
+      <c r="R187" s="1"/>
+      <c r="S187" s="1"/>
+      <c r="T187" s="1"/>
+      <c r="U187" s="1"/>
+      <c r="V187" s="1"/>
+      <c r="W187" s="1"/>
+      <c r="X187" s="1"/>
+      <c r="Y187" s="1"/>
+      <c r="Z187" s="1"/>
       <c r="AA187" s="1"/>
       <c r="AB187" s="1"/>
       <c r="AC187" s="1"/>
@@ -13430,214 +13504,236 @@
       <c r="AE187" s="1"/>
       <c r="AF187" s="1"/>
       <c r="AG187" s="1"/>
-      <c r="AH187" s="1"/>
-    </row>
-    <row r="188" spans="3:38" x14ac:dyDescent="0.3">
-      <c r="D188" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA188" s="1"/>
-      <c r="AB188" s="1"/>
-      <c r="AC188" s="1"/>
-      <c r="AD188" s="1"/>
-      <c r="AE188" s="1"/>
-      <c r="AF188" s="1"/>
-      <c r="AG188" s="1"/>
-      <c r="AH188" s="1"/>
+      <c r="AJ187" s="1"/>
+      <c r="AK187" s="15"/>
+      <c r="AL187" s="1"/>
+    </row>
+    <row r="188" spans="3:38" ht="32.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C188" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="D188" s="55"/>
+      <c r="E188" s="55"/>
+      <c r="F188" s="55"/>
+      <c r="G188" s="55"/>
+      <c r="H188" s="55"/>
+      <c r="I188" s="55"/>
+      <c r="J188" s="55"/>
+      <c r="K188" s="55"/>
+      <c r="L188" s="55"/>
+      <c r="M188" s="55"/>
+      <c r="N188" s="55"/>
+      <c r="O188" s="55"/>
+      <c r="P188" s="55"/>
+      <c r="Q188" s="55"/>
+      <c r="R188" s="55"/>
+      <c r="S188" s="55"/>
+      <c r="T188" s="55"/>
+      <c r="U188" s="55"/>
+      <c r="V188" s="55"/>
+      <c r="W188" s="55"/>
+      <c r="X188" s="55"/>
+      <c r="Y188" s="55"/>
+      <c r="Z188" s="55"/>
+      <c r="AA188" s="55"/>
+      <c r="AB188" s="55"/>
+      <c r="AC188" s="55"/>
+      <c r="AD188" s="55"/>
+      <c r="AE188" s="55"/>
+      <c r="AF188" s="55"/>
+      <c r="AG188" s="55"/>
+      <c r="AJ188" s="1"/>
+      <c r="AK188" s="1"/>
+      <c r="AL188" s="1"/>
     </row>
     <row r="189" spans="3:38" x14ac:dyDescent="0.3">
       <c r="AJ189" s="1"/>
       <c r="AK189" s="1"/>
       <c r="AL189" s="1"/>
     </row>
-    <row r="190" spans="3:38" x14ac:dyDescent="0.3">
+    <row r="190" spans="3:38" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="D190" s="25" t="s">
+        <v>255</v>
+      </c>
       <c r="AJ190" s="1"/>
       <c r="AK190" s="1"/>
       <c r="AL190" s="1"/>
     </row>
-    <row r="191" spans="3:38" x14ac:dyDescent="0.3">
+    <row r="191" spans="3:38" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="D191" s="25"/>
       <c r="AJ191" s="1"/>
       <c r="AK191" s="1"/>
       <c r="AL191" s="1"/>
     </row>
-    <row r="192" spans="3:38" x14ac:dyDescent="0.3">
-      <c r="C192" s="1"/>
-      <c r="D192" s="1"/>
-      <c r="E192" s="1"/>
-      <c r="F192" s="1"/>
-      <c r="G192" s="1"/>
-      <c r="H192" s="1"/>
-      <c r="I192" s="1"/>
-      <c r="J192" s="1"/>
-      <c r="K192" s="1"/>
-      <c r="L192" s="1"/>
-      <c r="M192" s="1"/>
-      <c r="N192" s="1"/>
-      <c r="O192" s="1"/>
-      <c r="P192" s="1"/>
-      <c r="Q192" s="1"/>
-      <c r="R192" s="1"/>
-      <c r="S192" s="1"/>
-      <c r="T192" s="1"/>
-      <c r="U192" s="1"/>
-      <c r="V192" s="1"/>
-      <c r="W192" s="1"/>
-      <c r="X192" s="1"/>
-      <c r="Y192" s="1"/>
-      <c r="Z192" s="1"/>
-      <c r="AA192" s="1"/>
-      <c r="AB192" s="1"/>
-      <c r="AC192" s="1"/>
-      <c r="AD192" s="1"/>
-      <c r="AE192" s="1"/>
-      <c r="AF192" s="1"/>
-      <c r="AG192" s="1"/>
+    <row r="192" spans="3:38" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D192" s="24" t="s">
+        <v>256</v>
+      </c>
       <c r="AJ192" s="1"/>
-      <c r="AK192" s="15"/>
+      <c r="AK192" s="1"/>
       <c r="AL192" s="1"/>
     </row>
-    <row r="193" spans="3:38" ht="32.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C193" s="54" t="s">
-        <v>81</v>
-      </c>
-      <c r="D193" s="55"/>
-      <c r="E193" s="55"/>
-      <c r="F193" s="55"/>
-      <c r="G193" s="55"/>
-      <c r="H193" s="55"/>
-      <c r="I193" s="55"/>
-      <c r="J193" s="55"/>
-      <c r="K193" s="55"/>
-      <c r="L193" s="55"/>
-      <c r="M193" s="55"/>
-      <c r="N193" s="55"/>
-      <c r="O193" s="55"/>
-      <c r="P193" s="55"/>
-      <c r="Q193" s="55"/>
-      <c r="R193" s="55"/>
-      <c r="S193" s="55"/>
-      <c r="T193" s="55"/>
-      <c r="U193" s="55"/>
-      <c r="V193" s="55"/>
-      <c r="W193" s="55"/>
-      <c r="X193" s="55"/>
-      <c r="Y193" s="55"/>
-      <c r="Z193" s="55"/>
-      <c r="AA193" s="55"/>
-      <c r="AB193" s="55"/>
-      <c r="AC193" s="55"/>
-      <c r="AD193" s="55"/>
-      <c r="AE193" s="55"/>
-      <c r="AF193" s="55"/>
-      <c r="AG193" s="55"/>
+    <row r="193" spans="4:38" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="D193" s="25"/>
       <c r="AJ193" s="1"/>
       <c r="AK193" s="1"/>
       <c r="AL193" s="1"/>
     </row>
-    <row r="194" spans="3:38" x14ac:dyDescent="0.3">
+    <row r="194" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="D194" s="53" t="s">
+        <v>250</v>
+      </c>
+      <c r="E194" s="53"/>
+      <c r="F194" s="53"/>
       <c r="AJ194" s="1"/>
       <c r="AK194" s="1"/>
       <c r="AL194" s="1"/>
     </row>
-    <row r="195" spans="3:38" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="D195" s="25" t="s">
-        <v>255</v>
-      </c>
+    <row r="195" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="D195" s="53" t="s">
+        <v>254</v>
+      </c>
+      <c r="E195" s="53"/>
+      <c r="F195" s="53"/>
       <c r="AJ195" s="1"/>
       <c r="AK195" s="1"/>
       <c r="AL195" s="1"/>
     </row>
-    <row r="196" spans="3:38" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="D196" s="25"/>
+    <row r="196" spans="4:38" x14ac:dyDescent="0.3">
       <c r="AJ196" s="1"/>
       <c r="AK196" s="1"/>
       <c r="AL196" s="1"/>
     </row>
-    <row r="197" spans="3:38" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="197" spans="4:38" ht="17.25" x14ac:dyDescent="0.3">
       <c r="D197" s="24" t="s">
-        <v>256</v>
+        <v>82</v>
       </c>
       <c r="AJ197" s="1"/>
       <c r="AK197" s="1"/>
       <c r="AL197" s="1"/>
     </row>
-    <row r="198" spans="3:38" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="D198" s="25"/>
+    <row r="198" spans="4:38" x14ac:dyDescent="0.3">
       <c r="AJ198" s="1"/>
       <c r="AK198" s="1"/>
       <c r="AL198" s="1"/>
     </row>
-    <row r="199" spans="3:38" x14ac:dyDescent="0.3">
-      <c r="D199" s="53" t="s">
-        <v>250</v>
-      </c>
-      <c r="E199" s="53"/>
-      <c r="F199" s="53"/>
+    <row r="199" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="D199" t="s">
+        <v>85</v>
+      </c>
       <c r="AJ199" s="1"/>
       <c r="AK199" s="1"/>
       <c r="AL199" s="1"/>
     </row>
-    <row r="200" spans="3:38" x14ac:dyDescent="0.3">
-      <c r="D200" s="53" t="s">
-        <v>254</v>
-      </c>
-      <c r="E200" s="53"/>
-      <c r="F200" s="53"/>
+    <row r="200" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="D200" t="s">
+        <v>83</v>
+      </c>
       <c r="AJ200" s="1"/>
       <c r="AK200" s="1"/>
       <c r="AL200" s="1"/>
     </row>
-    <row r="201" spans="3:38" x14ac:dyDescent="0.3">
+    <row r="201" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="D201" t="s">
+        <v>84</v>
+      </c>
       <c r="AJ201" s="1"/>
       <c r="AK201" s="1"/>
       <c r="AL201" s="1"/>
     </row>
-    <row r="202" spans="3:38" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D202" s="24" t="s">
-        <v>82</v>
-      </c>
+    <row r="202" spans="4:38" x14ac:dyDescent="0.3">
       <c r="AJ202" s="1"/>
       <c r="AK202" s="1"/>
       <c r="AL202" s="1"/>
     </row>
-    <row r="203" spans="3:38" x14ac:dyDescent="0.3">
+    <row r="203" spans="4:38" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D203" s="24" t="s">
+        <v>86</v>
+      </c>
       <c r="AJ203" s="1"/>
       <c r="AK203" s="1"/>
       <c r="AL203" s="1"/>
     </row>
-    <row r="204" spans="3:38" x14ac:dyDescent="0.3">
-      <c r="D204" t="s">
-        <v>85</v>
-      </c>
+    <row r="204" spans="4:38" x14ac:dyDescent="0.3">
       <c r="AJ204" s="1"/>
       <c r="AK204" s="1"/>
-      <c r="AL204" s="1"/>
-    </row>
-    <row r="205" spans="3:38" x14ac:dyDescent="0.3">
-      <c r="D205" t="s">
-        <v>83</v>
-      </c>
+      <c r="AL204" s="22"/>
+    </row>
+    <row r="205" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="D205" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E205" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="F205" s="32"/>
+      <c r="G205" s="32"/>
+      <c r="H205" s="32"/>
+      <c r="I205" s="33"/>
+      <c r="J205" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="K205" s="33"/>
+      <c r="AC205" s="18"/>
+      <c r="AF205" s="21"/>
       <c r="AJ205" s="1"/>
       <c r="AK205" s="1"/>
       <c r="AL205" s="1"/>
     </row>
-    <row r="206" spans="3:38" x14ac:dyDescent="0.3">
-      <c r="D206" t="s">
-        <v>84</v>
-      </c>
+    <row r="206" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="D206" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E206" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F206" s="6"/>
+      <c r="G206" s="6"/>
+      <c r="H206" s="6"/>
+      <c r="I206" s="7"/>
+      <c r="J206" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="K206" s="7"/>
+      <c r="AC206" s="19"/>
       <c r="AJ206" s="1"/>
       <c r="AK206" s="1"/>
       <c r="AL206" s="1"/>
     </row>
-    <row r="207" spans="3:38" x14ac:dyDescent="0.3">
+    <row r="207" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="D207" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E207" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F207" s="6"/>
+      <c r="G207" s="6"/>
+      <c r="H207" s="6"/>
+      <c r="I207" s="7"/>
+      <c r="J207" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K207" s="7"/>
       <c r="AJ207" s="1"/>
       <c r="AK207" s="1"/>
       <c r="AL207" s="1"/>
     </row>
-    <row r="208" spans="3:38" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D208" s="24" t="s">
-        <v>86</v>
-      </c>
+    <row r="208" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="D208" s="29" t="s">
+        <v>313</v>
+      </c>
+      <c r="E208" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F208" s="6"/>
+      <c r="G208" s="6"/>
+      <c r="H208" s="6"/>
+      <c r="I208" s="7"/>
+      <c r="J208" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K208" s="7"/>
       <c r="AJ208" s="1"/>
       <c r="AK208" s="1"/>
       <c r="AL208" s="1"/>
@@ -13645,1302 +13741,1231 @@
     <row r="209" spans="4:38" x14ac:dyDescent="0.3">
       <c r="AJ209" s="1"/>
       <c r="AK209" s="1"/>
-      <c r="AL209" s="22"/>
-    </row>
-    <row r="210" spans="4:38" x14ac:dyDescent="0.3">
-      <c r="D210" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E210" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="F210" s="32"/>
-      <c r="G210" s="32"/>
-      <c r="H210" s="32"/>
-      <c r="I210" s="33"/>
-      <c r="J210" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="K210" s="33"/>
-      <c r="AC210" s="18"/>
-      <c r="AF210" s="21"/>
+      <c r="AL209" s="1"/>
+    </row>
+    <row r="210" spans="4:38" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D210" s="24" t="s">
+        <v>96</v>
+      </c>
       <c r="AJ210" s="1"/>
       <c r="AK210" s="1"/>
       <c r="AL210" s="1"/>
     </row>
     <row r="211" spans="4:38" x14ac:dyDescent="0.3">
-      <c r="D211" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="E211" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F211" s="6"/>
-      <c r="G211" s="6"/>
-      <c r="H211" s="6"/>
-      <c r="I211" s="7"/>
-      <c r="J211" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="K211" s="7"/>
-      <c r="AC211" s="19"/>
       <c r="AJ211" s="1"/>
       <c r="AK211" s="1"/>
       <c r="AL211" s="1"/>
     </row>
     <row r="212" spans="4:38" x14ac:dyDescent="0.3">
-      <c r="D212" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="E212" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F212" s="6"/>
-      <c r="G212" s="6"/>
-      <c r="H212" s="6"/>
-      <c r="I212" s="7"/>
-      <c r="J212" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="K212" s="7"/>
+      <c r="D212" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="E212" s="33"/>
+      <c r="F212" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="G212" s="32"/>
+      <c r="H212" s="10"/>
+      <c r="I212" s="11"/>
+      <c r="Y212" s="20"/>
       <c r="AJ212" s="1"/>
       <c r="AK212" s="1"/>
-      <c r="AL212" s="1"/>
+      <c r="AL212" s="17"/>
     </row>
     <row r="213" spans="4:38" x14ac:dyDescent="0.3">
-      <c r="D213" s="29" t="s">
-        <v>314</v>
-      </c>
-      <c r="E213" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F213" s="6"/>
+      <c r="D213" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E213" s="7"/>
+      <c r="F213" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="G213" s="6"/>
       <c r="H213" s="6"/>
       <c r="I213" s="7"/>
-      <c r="J213" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="K213" s="7"/>
       <c r="AJ213" s="1"/>
       <c r="AK213" s="1"/>
       <c r="AL213" s="1"/>
     </row>
     <row r="214" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="D214" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E214" s="7"/>
+      <c r="F214" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G214" s="6"/>
+      <c r="H214" s="6"/>
+      <c r="I214" s="7"/>
       <c r="AJ214" s="1"/>
       <c r="AK214" s="1"/>
       <c r="AL214" s="1"/>
     </row>
-    <row r="215" spans="4:38" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D215" s="24" t="s">
-        <v>96</v>
-      </c>
+    <row r="215" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="D215" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="E215" s="7"/>
+      <c r="F215" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G215" s="6"/>
+      <c r="H215" s="6"/>
+      <c r="I215" s="7"/>
       <c r="AJ215" s="1"/>
-      <c r="AK215" s="1"/>
       <c r="AL215" s="1"/>
     </row>
     <row r="216" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="D216" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E216" s="4"/>
+      <c r="F216" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="G216" s="4"/>
+      <c r="H216" s="3"/>
+      <c r="I216" s="4"/>
       <c r="AJ216" s="1"/>
-      <c r="AK216" s="1"/>
+      <c r="AK216" s="22"/>
       <c r="AL216" s="1"/>
     </row>
     <row r="217" spans="4:38" x14ac:dyDescent="0.3">
-      <c r="D217" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="E217" s="33"/>
-      <c r="F217" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="G217" s="32"/>
-      <c r="H217" s="10"/>
-      <c r="I217" s="11"/>
-      <c r="Y217" s="20"/>
       <c r="AJ217" s="1"/>
       <c r="AK217" s="1"/>
-      <c r="AL217" s="17"/>
-    </row>
-    <row r="218" spans="4:38" x14ac:dyDescent="0.3">
-      <c r="D218" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E218" s="7"/>
-      <c r="F218" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G218" s="6"/>
-      <c r="H218" s="6"/>
-      <c r="I218" s="7"/>
+      <c r="AL217" s="1"/>
+    </row>
+    <row r="218" spans="4:38" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D218" s="24" t="s">
+        <v>314</v>
+      </c>
       <c r="AJ218" s="1"/>
-      <c r="AK218" s="1"/>
       <c r="AL218" s="1"/>
     </row>
     <row r="219" spans="4:38" x14ac:dyDescent="0.3">
-      <c r="D219" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E219" s="7"/>
-      <c r="F219" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G219" s="6"/>
-      <c r="H219" s="6"/>
-      <c r="I219" s="7"/>
+      <c r="AI219" s="20"/>
       <c r="AJ219" s="1"/>
-      <c r="AK219" s="1"/>
-      <c r="AL219" s="1"/>
+      <c r="AK219" s="22"/>
     </row>
     <row r="220" spans="4:38" x14ac:dyDescent="0.3">
-      <c r="D220" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="E220" s="7"/>
-      <c r="F220" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="G220" s="6"/>
-      <c r="H220" s="6"/>
-      <c r="I220" s="7"/>
+      <c r="D220" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI220" s="22"/>
       <c r="AJ220" s="1"/>
+      <c r="AK220" s="1"/>
       <c r="AL220" s="1"/>
     </row>
     <row r="221" spans="4:38" x14ac:dyDescent="0.3">
-      <c r="D221" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E221" s="4"/>
-      <c r="F221" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="G221" s="4"/>
-      <c r="H221" s="3"/>
-      <c r="I221" s="4"/>
+      <c r="D221" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="E221" t="s">
+        <v>108</v>
+      </c>
       <c r="AJ221" s="1"/>
-      <c r="AK221" s="22"/>
+      <c r="AK221" s="1"/>
       <c r="AL221" s="1"/>
     </row>
     <row r="222" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="E222" t="s">
+        <v>109</v>
+      </c>
       <c r="AJ222" s="1"/>
       <c r="AK222" s="1"/>
       <c r="AL222" s="1"/>
     </row>
-    <row r="223" spans="4:38" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D223" s="24" t="s">
+    <row r="223" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="E223" t="s">
+        <v>110</v>
+      </c>
+      <c r="AJ223" s="1"/>
+      <c r="AK223" s="1"/>
+      <c r="AL223" s="1"/>
+    </row>
+    <row r="224" spans="4:38" x14ac:dyDescent="0.3">
+      <c r="AJ224" s="1"/>
+      <c r="AK224" s="1"/>
+      <c r="AL224" s="1"/>
+    </row>
+    <row r="225" spans="4:17" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D225" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="227" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D227" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="228" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D228" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="231" spans="4:17" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D231" s="24" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="235" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="Q235" s="22" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="240" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="L240" s="21"/>
+    </row>
+    <row r="241" spans="13:36" x14ac:dyDescent="0.3">
+      <c r="M241" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="V241" s="22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="242" spans="13:36" x14ac:dyDescent="0.3">
+      <c r="M242" s="21"/>
+    </row>
+    <row r="246" spans="13:36" x14ac:dyDescent="0.3">
+      <c r="X246" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="250" spans="13:36" x14ac:dyDescent="0.3">
+      <c r="M250" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="251" spans="13:36" x14ac:dyDescent="0.3">
+      <c r="M251" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="252" spans="13:36" x14ac:dyDescent="0.3">
+      <c r="AB252" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ252" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="258" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="Q258" s="20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="263" spans="4:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D263" s="25" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="264" spans="4:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D264" s="25"/>
+    </row>
+    <row r="265" spans="4:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D265" s="24" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="266" spans="4:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D266" s="25"/>
+    </row>
+    <row r="267" spans="4:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D267" s="53" t="s">
+        <v>247</v>
+      </c>
+      <c r="E267" s="53"/>
+      <c r="F267" s="53"/>
+      <c r="G267" s="53"/>
+      <c r="H267" s="53"/>
+      <c r="I267" s="53"/>
+      <c r="J267" s="53"/>
+      <c r="K267" s="53"/>
+      <c r="L267" s="53"/>
+    </row>
+    <row r="268" spans="4:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D268" s="53" t="s">
+        <v>248</v>
+      </c>
+      <c r="E268" s="53"/>
+      <c r="F268" s="53"/>
+      <c r="G268" s="53"/>
+      <c r="H268" s="53"/>
+      <c r="I268" s="53"/>
+      <c r="J268" s="53"/>
+      <c r="K268" s="53"/>
+      <c r="L268" s="53"/>
+    </row>
+    <row r="269" spans="4:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D269" s="53" t="s">
+        <v>249</v>
+      </c>
+      <c r="E269" s="53"/>
+      <c r="F269" s="53"/>
+      <c r="G269" s="53"/>
+      <c r="H269" s="53"/>
+      <c r="I269" s="53"/>
+      <c r="J269" s="53"/>
+      <c r="K269" s="53"/>
+      <c r="L269" s="53"/>
+    </row>
+    <row r="270" spans="4:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D270" s="25"/>
+    </row>
+    <row r="271" spans="4:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D271" s="25"/>
+    </row>
+    <row r="273" spans="4:25" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D273" s="24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="275" spans="4:25" x14ac:dyDescent="0.3">
+      <c r="D275" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="281" spans="4:25" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D281" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="O281" s="12" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="283" spans="4:25" x14ac:dyDescent="0.3">
+      <c r="D283" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="E283" s="33"/>
+      <c r="F283" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="G283" s="32"/>
+      <c r="H283" s="33"/>
+      <c r="I283" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="J283" s="33"/>
+      <c r="K283" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="L283" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="M283" s="1"/>
+    </row>
+    <row r="284" spans="4:25" x14ac:dyDescent="0.3">
+      <c r="D284" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E284" s="7"/>
+      <c r="F284" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G284" s="6"/>
+      <c r="H284" s="7"/>
+      <c r="I284" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="J284" s="7"/>
+      <c r="K284" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="L284" s="29">
+        <v>1.35</v>
+      </c>
+      <c r="M284" s="1"/>
+      <c r="W284" s="52"/>
+      <c r="Y284" s="52"/>
+    </row>
+    <row r="285" spans="4:25" x14ac:dyDescent="0.3">
+      <c r="D285" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E285" s="7"/>
+      <c r="F285" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="G285" s="6"/>
+      <c r="H285" s="7"/>
+      <c r="I285" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="J285" s="7"/>
+      <c r="K285" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="L285" s="29">
+        <v>1.35</v>
+      </c>
+      <c r="M285" s="1"/>
+    </row>
+    <row r="286" spans="4:25" x14ac:dyDescent="0.3">
+      <c r="D286" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="E286" s="35"/>
+      <c r="F286" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="G286" s="1"/>
+      <c r="H286" s="35"/>
+      <c r="I286" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="J286" s="35"/>
+      <c r="K286" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="L286" s="29">
+        <v>1.35</v>
+      </c>
+      <c r="M286" s="1"/>
+      <c r="R286" s="28"/>
+      <c r="W286" s="28"/>
+      <c r="Y286" s="52" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="287" spans="4:25" x14ac:dyDescent="0.3">
+      <c r="D287" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E287" s="7"/>
+      <c r="F287" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G287" s="6"/>
+      <c r="H287" s="7"/>
+      <c r="I287" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="J287" s="7"/>
+      <c r="K287" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="L287" s="29">
+        <v>1.35</v>
+      </c>
+      <c r="M287" s="1"/>
+    </row>
+    <row r="288" spans="4:25" x14ac:dyDescent="0.3">
+      <c r="D288" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E288" s="4"/>
+      <c r="F288" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="G288" s="3"/>
+      <c r="H288" s="4"/>
+      <c r="I288" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J288" s="4"/>
+      <c r="K288" s="42" t="s">
+        <v>157</v>
+      </c>
+      <c r="L288" s="29">
+        <v>1.3</v>
+      </c>
+      <c r="M288" s="1"/>
+    </row>
+    <row r="290" spans="4:25" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D290" s="24" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="292" spans="4:25" x14ac:dyDescent="0.3">
+      <c r="D292" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="293" spans="4:25" x14ac:dyDescent="0.3">
+      <c r="E293" s="37"/>
+      <c r="Y293" s="52" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="294" spans="4:25" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D294" s="24" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="295" spans="4:25" x14ac:dyDescent="0.3">
+      <c r="W295" s="52"/>
+      <c r="Y295" s="52"/>
+    </row>
+    <row r="296" spans="4:25" x14ac:dyDescent="0.3">
+      <c r="D296" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="E296" s="49" t="s">
+        <v>164</v>
+      </c>
+      <c r="F296" s="50"/>
+      <c r="G296" s="51" t="s">
+        <v>142</v>
+      </c>
+      <c r="H296" s="33"/>
+      <c r="I296" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="J296" s="32"/>
+      <c r="K296" s="33"/>
+    </row>
+    <row r="297" spans="4:25" x14ac:dyDescent="0.3">
+      <c r="D297" s="38">
+        <v>1</v>
+      </c>
+      <c r="E297" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="F297" s="7"/>
+      <c r="G297" s="46" t="s">
+        <v>171</v>
+      </c>
+      <c r="H297" s="47"/>
+      <c r="I297" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="J297" s="6"/>
+      <c r="K297" s="7"/>
+    </row>
+    <row r="298" spans="4:25" x14ac:dyDescent="0.3">
+      <c r="D298" s="38">
+        <v>5</v>
+      </c>
+      <c r="E298" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="F298" s="7"/>
+      <c r="G298" s="46" t="s">
+        <v>172</v>
+      </c>
+      <c r="H298" s="47"/>
+      <c r="I298" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="J298" s="6"/>
+      <c r="K298" s="7"/>
+    </row>
+    <row r="299" spans="4:25" x14ac:dyDescent="0.3">
+      <c r="D299" s="38">
+        <v>10</v>
+      </c>
+      <c r="E299" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="F299" s="4"/>
+      <c r="G299" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="H299" s="39"/>
+      <c r="I299" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="J299" s="3"/>
+      <c r="K299" s="4"/>
+    </row>
+    <row r="301" spans="4:25" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D301" s="24" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="303" spans="4:25" x14ac:dyDescent="0.3">
+      <c r="D303" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="E303" s="33"/>
+      <c r="F303" s="33" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="304" spans="4:25" x14ac:dyDescent="0.3">
+      <c r="D304" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="E304" s="7"/>
+      <c r="F304" s="29" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="305" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D305" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E305" s="7"/>
+      <c r="F305" s="29" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="306" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D306" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E306" s="7"/>
+      <c r="F306" s="29" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="311" spans="4:14" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="D311" s="25" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="312" spans="4:14" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="D312" s="25"/>
+    </row>
+    <row r="313" spans="4:14" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D313" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="AJ223" s="1"/>
-      <c r="AL223" s="1"/>
-    </row>
-    <row r="224" spans="4:38" x14ac:dyDescent="0.3">
-      <c r="AI224" s="20"/>
-      <c r="AJ224" s="1"/>
-      <c r="AK224" s="22"/>
-    </row>
-    <row r="225" spans="4:38" x14ac:dyDescent="0.3">
-      <c r="D225" t="s">
-        <v>106</v>
-      </c>
-      <c r="AI225" s="22"/>
-      <c r="AJ225" s="1"/>
-      <c r="AK225" s="1"/>
-      <c r="AL225" s="1"/>
-    </row>
-    <row r="226" spans="4:38" x14ac:dyDescent="0.3">
-      <c r="D226" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="E226" t="s">
-        <v>108</v>
-      </c>
-      <c r="AJ226" s="1"/>
-      <c r="AK226" s="1"/>
-      <c r="AL226" s="1"/>
-    </row>
-    <row r="227" spans="4:38" x14ac:dyDescent="0.3">
-      <c r="E227" t="s">
-        <v>109</v>
-      </c>
-      <c r="AJ227" s="1"/>
-      <c r="AK227" s="1"/>
-      <c r="AL227" s="1"/>
-    </row>
-    <row r="228" spans="4:38" x14ac:dyDescent="0.3">
-      <c r="E228" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ228" s="1"/>
-      <c r="AK228" s="1"/>
-      <c r="AL228" s="1"/>
-    </row>
-    <row r="229" spans="4:38" x14ac:dyDescent="0.3">
-      <c r="AJ229" s="1"/>
-      <c r="AK229" s="1"/>
-      <c r="AL229" s="1"/>
-    </row>
-    <row r="230" spans="4:38" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D230" s="24" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="232" spans="4:38" x14ac:dyDescent="0.3">
-      <c r="D232" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="233" spans="4:38" x14ac:dyDescent="0.3">
-      <c r="D233" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="236" spans="4:38" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D236" s="24" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="240" spans="4:38" x14ac:dyDescent="0.3">
-      <c r="Q240" s="22" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="245" spans="12:24" x14ac:dyDescent="0.3">
-      <c r="L245" s="21"/>
-    </row>
-    <row r="246" spans="12:24" x14ac:dyDescent="0.3">
-      <c r="M246" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="V246" s="22" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="247" spans="12:24" x14ac:dyDescent="0.3">
-      <c r="M247" s="21"/>
-    </row>
-    <row r="251" spans="12:24" x14ac:dyDescent="0.3">
-      <c r="X251" s="21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="255" spans="12:24" x14ac:dyDescent="0.3">
-      <c r="M255" s="18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="256" spans="12:24" x14ac:dyDescent="0.3">
-      <c r="M256" s="19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="257" spans="4:36" x14ac:dyDescent="0.3">
-      <c r="AB257" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="AJ257" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="263" spans="4:36" x14ac:dyDescent="0.3">
-      <c r="Q263" s="20" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="268" spans="4:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D268" s="25" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="269" spans="4:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D269" s="25"/>
-    </row>
-    <row r="270" spans="4:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D270" s="24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="271" spans="4:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D271" s="25"/>
-    </row>
-    <row r="272" spans="4:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D272" s="53" t="s">
-        <v>247</v>
-      </c>
-      <c r="E272" s="53"/>
-      <c r="F272" s="53"/>
-      <c r="G272" s="53"/>
-      <c r="H272" s="53"/>
-      <c r="I272" s="53"/>
-      <c r="J272" s="53"/>
-      <c r="K272" s="53"/>
-      <c r="L272" s="53"/>
-    </row>
-    <row r="273" spans="4:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D273" s="53" t="s">
-        <v>248</v>
-      </c>
-      <c r="E273" s="53"/>
-      <c r="F273" s="53"/>
-      <c r="G273" s="53"/>
-      <c r="H273" s="53"/>
-      <c r="I273" s="53"/>
-      <c r="J273" s="53"/>
-      <c r="K273" s="53"/>
-      <c r="L273" s="53"/>
-    </row>
-    <row r="274" spans="4:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D274" s="53" t="s">
-        <v>249</v>
-      </c>
-      <c r="E274" s="53"/>
-      <c r="F274" s="53"/>
-      <c r="G274" s="53"/>
-      <c r="H274" s="53"/>
-      <c r="I274" s="53"/>
-      <c r="J274" s="53"/>
-      <c r="K274" s="53"/>
-      <c r="L274" s="53"/>
-    </row>
-    <row r="275" spans="4:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D275" s="25"/>
-    </row>
-    <row r="276" spans="4:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D276" s="25"/>
-    </row>
-    <row r="278" spans="4:15" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D278" s="24" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="280" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D280" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="286" spans="4:15" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D286" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="O286" s="12" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="288" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D288" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="E288" s="33"/>
-      <c r="F288" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="G288" s="32"/>
-      <c r="H288" s="33"/>
-      <c r="I288" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="J288" s="33"/>
-      <c r="K288" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="L288" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="M288" s="1"/>
-    </row>
-    <row r="289" spans="4:25" x14ac:dyDescent="0.3">
-      <c r="D289" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="E289" s="7"/>
-      <c r="F289" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="G289" s="6"/>
-      <c r="H289" s="7"/>
-      <c r="I289" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="J289" s="7"/>
-      <c r="K289" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="L289" s="29">
-        <v>1.35</v>
-      </c>
-      <c r="M289" s="1"/>
-      <c r="W289" s="52"/>
-      <c r="Y289" s="52"/>
-    </row>
-    <row r="290" spans="4:25" x14ac:dyDescent="0.3">
-      <c r="D290" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="E290" s="7"/>
-      <c r="F290" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="G290" s="6"/>
-      <c r="H290" s="7"/>
-      <c r="I290" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="J290" s="7"/>
-      <c r="K290" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="L290" s="29">
-        <v>1.35</v>
-      </c>
-      <c r="M290" s="1"/>
-    </row>
-    <row r="291" spans="4:25" x14ac:dyDescent="0.3">
-      <c r="D291" s="34" t="s">
-        <v>142</v>
-      </c>
-      <c r="E291" s="35"/>
-      <c r="F291" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="G291" s="1"/>
-      <c r="H291" s="35"/>
-      <c r="I291" s="34" t="s">
-        <v>150</v>
-      </c>
-      <c r="J291" s="35"/>
-      <c r="K291" s="41" t="s">
-        <v>156</v>
-      </c>
-      <c r="L291" s="29">
-        <v>1.35</v>
-      </c>
-      <c r="M291" s="1"/>
-      <c r="R291" s="28"/>
-      <c r="W291" s="28"/>
-      <c r="Y291" s="52" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="292" spans="4:25" x14ac:dyDescent="0.3">
-      <c r="D292" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="E292" s="7"/>
-      <c r="F292" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="G292" s="6"/>
-      <c r="H292" s="7"/>
-      <c r="I292" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="J292" s="7"/>
-      <c r="K292" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="L292" s="29">
-        <v>1.35</v>
-      </c>
-      <c r="M292" s="1"/>
-    </row>
-    <row r="293" spans="4:25" x14ac:dyDescent="0.3">
-      <c r="D293" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E293" s="4"/>
-      <c r="F293" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="G293" s="3"/>
-      <c r="H293" s="4"/>
-      <c r="I293" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="J293" s="4"/>
-      <c r="K293" s="42" t="s">
-        <v>157</v>
-      </c>
-      <c r="L293" s="29">
-        <v>1.3</v>
-      </c>
-      <c r="M293" s="1"/>
-    </row>
-    <row r="295" spans="4:25" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D295" s="24" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="297" spans="4:25" x14ac:dyDescent="0.3">
-      <c r="D297" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="298" spans="4:25" x14ac:dyDescent="0.3">
-      <c r="E298" s="37"/>
-      <c r="Y298" s="52" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="299" spans="4:25" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D299" s="24" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="300" spans="4:25" x14ac:dyDescent="0.3">
-      <c r="W300" s="52"/>
-      <c r="Y300" s="52"/>
-    </row>
-    <row r="301" spans="4:25" x14ac:dyDescent="0.3">
-      <c r="D301" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="E301" s="49" t="s">
-        <v>164</v>
-      </c>
-      <c r="F301" s="50"/>
-      <c r="G301" s="51" t="s">
-        <v>142</v>
-      </c>
-      <c r="H301" s="33"/>
-      <c r="I301" s="32" t="s">
-        <v>174</v>
-      </c>
-      <c r="J301" s="32"/>
-      <c r="K301" s="33"/>
-    </row>
-    <row r="302" spans="4:25" x14ac:dyDescent="0.3">
-      <c r="D302" s="38">
+    </row>
+    <row r="314" spans="4:14" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="D314" s="25"/>
+    </row>
+    <row r="315" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D315" s="53" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="316" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D316" s="53" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="317" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D317" s="53" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="319" spans="4:14" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D319" s="24" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="320" spans="4:14" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="N320" s="24" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="321" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D321" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="E321" s="32"/>
+      <c r="F321" s="32"/>
+      <c r="G321" s="31" t="s">
+        <v>193</v>
+      </c>
+      <c r="H321" s="32"/>
+      <c r="I321" s="32"/>
+      <c r="J321" s="32"/>
+      <c r="K321" s="33"/>
+    </row>
+    <row r="322" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D322" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E322" s="6"/>
+      <c r="F322" s="7"/>
+      <c r="G322" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="H322" s="6"/>
+      <c r="I322" s="6"/>
+      <c r="J322" s="6"/>
+      <c r="K322" s="7"/>
+    </row>
+    <row r="323" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D323" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="E323" s="6"/>
+      <c r="F323" s="7"/>
+      <c r="G323" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="H323" s="6"/>
+      <c r="I323" s="6"/>
+      <c r="J323" s="6"/>
+      <c r="K323" s="7"/>
+    </row>
+    <row r="325" spans="4:11" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D325" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="327" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D327" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="329" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D329" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="E329" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="F329" s="30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="330" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D330" s="38">
         <v>1</v>
       </c>
-      <c r="E302" s="45" t="s">
-        <v>168</v>
-      </c>
-      <c r="F302" s="7"/>
-      <c r="G302" s="46" t="s">
-        <v>171</v>
-      </c>
-      <c r="H302" s="47"/>
-      <c r="I302" s="48" t="s">
-        <v>166</v>
-      </c>
-      <c r="J302" s="6"/>
-      <c r="K302" s="7"/>
-    </row>
-    <row r="303" spans="4:25" x14ac:dyDescent="0.3">
-      <c r="D303" s="38">
+      <c r="E330" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="F330" s="29" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="331" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D331" s="38">
+        <v>2</v>
+      </c>
+      <c r="E331" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="F331" s="29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="332" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D332" s="38">
+        <v>3</v>
+      </c>
+      <c r="E332" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="F332" s="29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="333" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D333" s="38">
+        <v>4</v>
+      </c>
+      <c r="E333" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="F333" s="29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="334" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D334" s="38">
         <v>5</v>
       </c>
-      <c r="E303" s="45" t="s">
-        <v>169</v>
-      </c>
-      <c r="F303" s="7"/>
-      <c r="G303" s="46" t="s">
-        <v>172</v>
-      </c>
-      <c r="H303" s="47"/>
-      <c r="I303" s="48" t="s">
-        <v>165</v>
-      </c>
-      <c r="J303" s="6"/>
-      <c r="K303" s="7"/>
-    </row>
-    <row r="304" spans="4:25" x14ac:dyDescent="0.3">
-      <c r="D304" s="38">
+      <c r="E334" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="F334" s="29" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="335" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D335" s="38">
+        <v>6</v>
+      </c>
+      <c r="E335" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="F335" s="29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="336" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D336" s="38">
+        <v>7</v>
+      </c>
+      <c r="E336" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="F336" s="29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="337" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D337" s="38">
+        <v>8</v>
+      </c>
+      <c r="E337" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="F337" s="29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="338" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D338" s="38">
+        <v>9</v>
+      </c>
+      <c r="E338" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="F338" s="29" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="339" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D339" s="38">
         <v>10</v>
       </c>
-      <c r="E304" s="44" t="s">
-        <v>170</v>
-      </c>
-      <c r="F304" s="4"/>
-      <c r="G304" s="46" t="s">
-        <v>173</v>
-      </c>
-      <c r="H304" s="39"/>
-      <c r="I304" s="43" t="s">
-        <v>167</v>
-      </c>
-      <c r="J304" s="3"/>
-      <c r="K304" s="4"/>
-    </row>
-    <row r="306" spans="4:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D306" s="24" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="308" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D308" s="31" t="s">
-        <v>177</v>
-      </c>
-      <c r="E308" s="33"/>
-      <c r="F308" s="33" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="309" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D309" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="E309" s="7"/>
-      <c r="F309" s="29" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="310" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D310" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="E310" s="7"/>
-      <c r="F310" s="29" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="311" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D311" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="E311" s="7"/>
-      <c r="F311" s="29" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="316" spans="4:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="D316" s="25" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="317" spans="4:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="D317" s="25"/>
-    </row>
-    <row r="318" spans="4:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D318" s="24" t="s">
+      <c r="E339" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="F339" s="29" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="340" spans="4:15" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="N340" s="24" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="341" spans="4:15" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D341" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="O341" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="342" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="O342" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="343" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D343" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="E343" s="33"/>
+      <c r="F343" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="G343" s="32"/>
+      <c r="H343" s="32"/>
+      <c r="I343" s="33"/>
+    </row>
+    <row r="344" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D344" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="E344" s="7"/>
+      <c r="F344" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="G344" s="6"/>
+      <c r="H344" s="6"/>
+      <c r="I344" s="7"/>
+    </row>
+    <row r="345" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D345" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E345" s="7"/>
+      <c r="F345" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="G345" s="6"/>
+      <c r="H345" s="6"/>
+      <c r="I345" s="7"/>
+    </row>
+    <row r="346" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D346" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E346" s="7"/>
+      <c r="F346" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="G346" s="6"/>
+      <c r="H346" s="6"/>
+      <c r="I346" s="7"/>
+    </row>
+    <row r="347" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D347" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E347" s="7"/>
+      <c r="F347" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="G347" s="6"/>
+      <c r="H347" s="6"/>
+      <c r="I347" s="7"/>
+    </row>
+    <row r="348" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D348" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E348" s="4"/>
+      <c r="F348" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G348" s="3"/>
+      <c r="H348" s="3"/>
+      <c r="I348" s="4"/>
+    </row>
+    <row r="353" spans="4:22" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="D353" s="25" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="355" spans="4:22" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D355" s="24" t="s">
+        <v>298</v>
+      </c>
+      <c r="L355" s="24" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="357" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="D357" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="358" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="D358" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="359" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="D359" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="361" spans="4:22" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D361" s="24" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="362" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="V362" s="20" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="363" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="D363" s="31" t="s">
+        <v>301</v>
+      </c>
+      <c r="E363" s="33"/>
+      <c r="F363" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="G363" s="32"/>
+      <c r="H363" s="30" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="364" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="D364" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E364" s="6"/>
+      <c r="F364" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="G364" s="7"/>
+      <c r="H364" s="7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="365" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="D365" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E365" s="6"/>
+      <c r="F365" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="G365" s="7"/>
+      <c r="H365" s="7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="366" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="D366" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="E366" s="6"/>
+      <c r="F366" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="G366" s="7"/>
+      <c r="H366" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="367" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="D367" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E367" s="3"/>
+      <c r="F367" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G367" s="4"/>
+      <c r="H367" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="369" spans="4:27" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D369" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="AA369" s="20" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="370" spans="4:27" x14ac:dyDescent="0.3">
+      <c r="V370" s="20" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="371" spans="4:27" x14ac:dyDescent="0.3">
+      <c r="D371" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="372" spans="4:27" x14ac:dyDescent="0.3">
+      <c r="D372" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="373" spans="4:27" x14ac:dyDescent="0.3">
+      <c r="D373" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="374" spans="4:27" x14ac:dyDescent="0.3">
+      <c r="D374" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="319" spans="4:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="D319" s="25"/>
-    </row>
-    <row r="320" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D320" s="53" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="321" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D321" s="53" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="322" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D322" s="53" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="324" spans="4:14" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D324" s="24" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="325" spans="4:14" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="N325" s="24" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="326" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D326" s="31" t="s">
-        <v>190</v>
-      </c>
-      <c r="E326" s="32"/>
-      <c r="F326" s="32"/>
-      <c r="G326" s="31" t="s">
-        <v>193</v>
-      </c>
-      <c r="H326" s="32"/>
-      <c r="I326" s="32"/>
-      <c r="J326" s="32"/>
-      <c r="K326" s="33"/>
-    </row>
-    <row r="327" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D327" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="E327" s="6"/>
-      <c r="F327" s="7"/>
-      <c r="G327" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="H327" s="6"/>
-      <c r="I327" s="6"/>
-      <c r="J327" s="6"/>
-      <c r="K327" s="7"/>
-    </row>
-    <row r="328" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D328" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="E328" s="6"/>
-      <c r="F328" s="7"/>
-      <c r="G328" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="H328" s="6"/>
-      <c r="I328" s="6"/>
-      <c r="J328" s="6"/>
-      <c r="K328" s="7"/>
-    </row>
-    <row r="330" spans="4:14" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D330" s="24" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="332" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D332" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="334" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D334" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="E334" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="F334" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="335" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D335" s="38">
-        <v>1</v>
-      </c>
-      <c r="E335" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="F335" s="29" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="336" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D336" s="38">
-        <v>2</v>
-      </c>
-      <c r="E336" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="F336" s="29" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="337" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D337" s="38">
-        <v>3</v>
-      </c>
-      <c r="E337" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="F337" s="29" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="338" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D338" s="38">
-        <v>4</v>
-      </c>
-      <c r="E338" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="F338" s="29" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="339" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D339" s="38">
-        <v>5</v>
-      </c>
-      <c r="E339" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="F339" s="29" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="340" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D340" s="38">
-        <v>6</v>
-      </c>
-      <c r="E340" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="F340" s="29" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="341" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D341" s="38">
-        <v>7</v>
-      </c>
-      <c r="E341" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="F341" s="29" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="342" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D342" s="38">
-        <v>8</v>
-      </c>
-      <c r="E342" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="F342" s="29" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="343" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D343" s="38">
-        <v>9</v>
-      </c>
-      <c r="E343" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="F343" s="29" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="344" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D344" s="38">
-        <v>10</v>
-      </c>
-      <c r="E344" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="F344" s="29" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="346" spans="4:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D346" s="24" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="348" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D348" s="31" t="s">
-        <v>198</v>
-      </c>
-      <c r="E348" s="33"/>
-      <c r="F348" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="G348" s="32"/>
-      <c r="H348" s="32"/>
-      <c r="I348" s="33"/>
-    </row>
-    <row r="349" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D349" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="E349" s="7"/>
-      <c r="F349" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="G349" s="6"/>
-      <c r="H349" s="6"/>
-      <c r="I349" s="7"/>
-    </row>
-    <row r="350" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D350" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="E350" s="7"/>
-      <c r="F350" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="G350" s="6"/>
-      <c r="H350" s="6"/>
-      <c r="I350" s="7"/>
-    </row>
-    <row r="351" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D351" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="E351" s="7"/>
-      <c r="F351" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="G351" s="6"/>
-      <c r="H351" s="6"/>
-      <c r="I351" s="7"/>
-    </row>
-    <row r="352" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D352" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="E352" s="7"/>
-      <c r="F352" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="G352" s="6"/>
-      <c r="H352" s="6"/>
-      <c r="I352" s="7"/>
-    </row>
-    <row r="353" spans="4:22" x14ac:dyDescent="0.3">
-      <c r="D353" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E353" s="4"/>
-      <c r="F353" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="G353" s="3"/>
-      <c r="H353" s="3"/>
-      <c r="I353" s="4"/>
-    </row>
-    <row r="358" spans="4:22" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="D358" s="25" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="360" spans="4:22" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D360" s="24" t="s">
-        <v>298</v>
-      </c>
-      <c r="L360" s="24" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="362" spans="4:22" x14ac:dyDescent="0.3">
-      <c r="D362" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="363" spans="4:22" x14ac:dyDescent="0.3">
-      <c r="D363" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="364" spans="4:22" x14ac:dyDescent="0.3">
-      <c r="D364" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="366" spans="4:22" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D366" s="24" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="367" spans="4:22" x14ac:dyDescent="0.3">
-      <c r="V367" s="20" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="368" spans="4:22" x14ac:dyDescent="0.3">
-      <c r="D368" s="31" t="s">
-        <v>301</v>
-      </c>
-      <c r="E368" s="33"/>
-      <c r="F368" s="32" t="s">
-        <v>211</v>
-      </c>
-      <c r="G368" s="32"/>
-      <c r="H368" s="30" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="369" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="D369" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E369" s="6"/>
-      <c r="F369" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="G369" s="7"/>
-      <c r="H369" s="7" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="370" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="D370" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="E370" s="6"/>
-      <c r="F370" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="G370" s="7"/>
-      <c r="H370" s="7" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="371" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="D371" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="E371" s="6"/>
-      <c r="F371" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="G371" s="7"/>
-      <c r="H371" s="7" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="372" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="D372" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="E372" s="3"/>
-      <c r="F372" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="G372" s="4"/>
-      <c r="H372" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="374" spans="4:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D374" s="24" t="s">
-        <v>228</v>
-      </c>
-      <c r="AA374" s="20" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="375" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="V375" s="20" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="376" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="D376" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="377" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="D377" t="s">
-        <v>229</v>
+    <row r="376" spans="4:27" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D376" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="AA376" s="20" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="378" spans="4:27" x14ac:dyDescent="0.3">
       <c r="D378" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="379" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="D379" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="381" spans="4:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D381" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="AA381" s="20" t="s">
-        <v>242</v>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="380" spans="4:27" x14ac:dyDescent="0.3">
+      <c r="D380" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="E380" s="30" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="381" spans="4:27" x14ac:dyDescent="0.3">
+      <c r="D381" s="38">
+        <v>1</v>
+      </c>
+      <c r="E381" s="29" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="382" spans="4:27" x14ac:dyDescent="0.3">
+      <c r="D382" s="38">
+        <v>2</v>
+      </c>
+      <c r="E382" s="29" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="383" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="D383" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="385" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D385" s="30" t="s">
-        <v>232</v>
-      </c>
-      <c r="E385" s="30" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="386" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D386" s="38">
-        <v>1</v>
-      </c>
-      <c r="E386" s="29" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="387" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D387" s="38">
-        <v>2</v>
-      </c>
-      <c r="E387" s="29" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="388" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D388" s="38">
+      <c r="D383" s="38">
         <v>3</v>
       </c>
-      <c r="E388" s="29" t="s">
+      <c r="E383" s="29" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="389" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D389" s="38">
+    <row r="384" spans="4:27" x14ac:dyDescent="0.3">
+      <c r="D384" s="38">
         <v>4</v>
       </c>
-      <c r="E389" s="29" t="s">
+      <c r="E384" s="29" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="390" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D390" s="38">
+    <row r="385" spans="4:29" x14ac:dyDescent="0.3">
+      <c r="D385" s="38">
         <v>5</v>
       </c>
-      <c r="E390" s="29" t="s">
+      <c r="E385" s="29" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="395" spans="4:12" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="D395" s="25" t="s">
+    <row r="390" spans="4:29" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="D390" s="25" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="397" spans="4:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D397" s="24" t="s">
+    <row r="392" spans="4:29" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D392" s="24" t="s">
         <v>257</v>
       </c>
-      <c r="L397" s="24" t="s">
+      <c r="L392" s="24" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="399" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D399" t="s">
+    <row r="394" spans="4:29" x14ac:dyDescent="0.3">
+      <c r="D394" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="400" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="395" spans="4:29" x14ac:dyDescent="0.3">
+      <c r="D395" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="396" spans="4:29" x14ac:dyDescent="0.3">
+      <c r="D396" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="398" spans="4:29" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D398" s="24" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC398" s="20" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="400" spans="4:29" x14ac:dyDescent="0.3">
       <c r="D400" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="401" spans="4:29" x14ac:dyDescent="0.3">
       <c r="D401" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="403" spans="4:29" ht="17.25" x14ac:dyDescent="0.3">
       <c r="D403" s="24" t="s">
-        <v>261</v>
-      </c>
-      <c r="AC403" s="20" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
     </row>
     <row r="405" spans="4:29" x14ac:dyDescent="0.3">
-      <c r="D405" t="s">
-        <v>263</v>
+      <c r="D405" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="E405" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="AC405" s="20" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="406" spans="4:29" x14ac:dyDescent="0.3">
-      <c r="D406" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="408" spans="4:29" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D408" s="24" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="410" spans="4:29" x14ac:dyDescent="0.3">
-      <c r="D410" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="E410" s="30" t="s">
-        <v>268</v>
-      </c>
-      <c r="AC410" s="20" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="411" spans="4:29" x14ac:dyDescent="0.3">
-      <c r="D411" s="29" t="s">
+      <c r="D406" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="E411" s="29">
+      <c r="E406" s="29">
         <v>200</v>
       </c>
     </row>
-    <row r="412" spans="4:29" x14ac:dyDescent="0.3">
-      <c r="D412" s="29" t="s">
+    <row r="407" spans="4:29" x14ac:dyDescent="0.3">
+      <c r="D407" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="E412" s="29">
+      <c r="E407" s="29">
         <v>15</v>
       </c>
     </row>
+    <row r="408" spans="4:29" x14ac:dyDescent="0.3">
+      <c r="D408" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="E408" s="29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="409" spans="4:29" x14ac:dyDescent="0.3">
+      <c r="D409" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="E409" s="29">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="411" spans="4:29" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D411" s="24" t="s">
+        <v>269</v>
+      </c>
+    </row>
     <row r="413" spans="4:29" x14ac:dyDescent="0.3">
-      <c r="D413" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="E413" s="29">
-        <v>8</v>
-      </c>
+      <c r="D413" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="E413" s="33"/>
+      <c r="F413" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="G413" s="32"/>
+      <c r="H413" s="33"/>
     </row>
     <row r="414" spans="4:29" x14ac:dyDescent="0.3">
-      <c r="D414" s="29" t="s">
-        <v>267</v>
-      </c>
-      <c r="E414" s="29">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="416" spans="4:29" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D416" s="24" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="418" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D418" s="31" t="s">
-        <v>177</v>
-      </c>
-      <c r="E418" s="33"/>
-      <c r="F418" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="G418" s="32"/>
-      <c r="H418" s="33"/>
-    </row>
-    <row r="419" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D419" s="5" t="s">
+      <c r="D414" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="E419" s="7"/>
-      <c r="F419" s="6" t="s">
+      <c r="E414" s="7"/>
+      <c r="F414" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="G419" s="6"/>
-      <c r="H419" s="7"/>
-    </row>
-    <row r="420" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D420" s="5" t="s">
+      <c r="G414" s="6"/>
+      <c r="H414" s="7"/>
+    </row>
+    <row r="415" spans="4:29" x14ac:dyDescent="0.3">
+      <c r="D415" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="E420" s="7"/>
-      <c r="F420" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="G420" s="6"/>
-      <c r="H420" s="7"/>
-    </row>
-    <row r="421" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D421" s="5" t="s">
+      <c r="E415" s="7"/>
+      <c r="F415" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="G415" s="6"/>
+      <c r="H415" s="7"/>
+    </row>
+    <row r="416" spans="4:29" x14ac:dyDescent="0.3">
+      <c r="D416" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="E421" s="7"/>
-      <c r="F421" s="6" t="s">
+      <c r="E416" s="7"/>
+      <c r="F416" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="G421" s="6"/>
-      <c r="H421" s="7"/>
-    </row>
-    <row r="422" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D422" s="2" t="s">
+      <c r="G416" s="6"/>
+      <c r="H416" s="7"/>
+    </row>
+    <row r="417" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D417" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="E422" s="4"/>
-      <c r="F422" s="3" t="s">
+      <c r="E417" s="4"/>
+      <c r="F417" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="G422" s="3"/>
-      <c r="H422" s="4"/>
+      <c r="G417" s="3"/>
+      <c r="H417" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>